<commit_message>
Remove break at sd error
</commit_message>
<xml_diff>
--- a/gals_mini.xlsx
+++ b/gals_mini.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,14 +434,134 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Download Status</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DiffusionStatus1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Take1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Shot1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Style1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Hero1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>URL1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DiffusionStatus2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Take2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Shot2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Style2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Hero2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>URL2</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>DiffusionStatus3</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Take3</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Shot3</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Style3</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Hero3</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>URL3</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>DiffusionStatus4</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Take4</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Shot4</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Style4</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Hero4</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>URL4</t>
         </is>
       </c>
     </row>
@@ -444,6 +576,62 @@
           <t>Success</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AzuletteCosplay</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>manga</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>blonde</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>pop-art</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -456,6 +644,94 @@
           <t>Success</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>skirt</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>art nouveau</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>front-mediumshot</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>akira toriyama</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blonde</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>cheer</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>watercolor</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>4</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>front-mediumshot4</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>painting</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>blonde</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -468,6 +744,90 @@
           <t>Success</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>profile-mediumshot</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>art nouveau</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>BelindaPop</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>watercolor</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>whore</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>front-mediumshotdown</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>pop-art</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>4</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>nude-squat-9</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>alphonse mucha style</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -480,6 +840,48 @@
           <t>Success</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>front-medium-arms</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>comic-book</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>blonde</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -492,6 +894,90 @@
           <t>Success</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>AzuletteCosplay</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>akira toriyama</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>dancing</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>lineart</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>brunette</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>DamarizGonzalez</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>japanese-animation</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>profile-mediumshot</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>pin-up</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>